<commit_message>
fix column types issue
</commit_message>
<xml_diff>
--- a/excelPath/test/testChartModule2Excel.xlsx
+++ b/excelPath/test/testChartModule2Excel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>name(string)</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>13:01:30.123</t>
-  </si>
-  <si>
-    <t>500.5</t>
   </si>
   <si>
     <t>2006-04-19</t>
@@ -530,46 +527,46 @@
       <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>500.5</v>
+      </c>
+      <c r="E3" t="s">
         <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
       </c>
       <c r="F3">
         <v>27</v>
       </c>
       <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
         <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>600</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4">
         <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>